<commit_message>
updated requirements.txt, and Manual GUI Tests.xlsx
</commit_message>
<xml_diff>
--- a/Manual GUI Tests.xlsx
+++ b/Manual GUI Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\DMatveevAPIProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456BF00A-FBF9-40E7-B8B8-993DC10AC298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB554A77-D9EB-4DB4-807D-D5520A315D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t xml:space="preserve">Dennis </t>
   </si>
@@ -33,15 +33,6 @@
     <t>Matveev</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>GUI</t>
-  </si>
-  <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Test Case Description</t>
   </si>
   <si>
@@ -57,7 +48,100 @@
     <t>Expected Results</t>
   </si>
   <si>
-    <t>.</t>
+    <t>Exit Program</t>
+  </si>
+  <si>
+    <t>Window Closes</t>
+  </si>
+  <si>
+    <t>Run Program</t>
+  </si>
+  <si>
+    <t>Update Api Data</t>
+  </si>
+  <si>
+    <t>Api Data Collected, Task Successful Displayed</t>
+  </si>
+  <si>
+    <t>Window should Close</t>
+  </si>
+  <si>
+    <t>A pop up message that says task completed</t>
+  </si>
+  <si>
+    <t>Update Xls Data</t>
+  </si>
+  <si>
+    <t>Prompts User to select Xls file, message that task is completed</t>
+  </si>
+  <si>
+    <t>Ask user to select file, Pop up message that task is completed</t>
+  </si>
+  <si>
+    <t>Visualize Grads vs Jobs Data Ascending List</t>
+  </si>
+  <si>
+    <t>Visualize Grads vs Jobs Data Descending List</t>
+  </si>
+  <si>
+    <t>Visualize Bal vs Salary Data Ascending List</t>
+  </si>
+  <si>
+    <t>Visualize Bal vs Salary Data Descending List</t>
+  </si>
+  <si>
+    <t>Visualizee Bal vs Salary Map</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                      2. Click 'Compare 3YearCohortBal vs 25PercentileSalary per state'       3. Click 'Visualize TXT Format' 4. Click 'Ascending Order'</t>
+  </si>
+  <si>
+    <t>1. Click 'Exit'                                                                                                                     2. Click 'Exit</t>
+  </si>
+  <si>
+    <t>1. Click 'Update'                                                                                                          2. Click ' Update Api DB'</t>
+  </si>
+  <si>
+    <t>1. Click 'Update'                                                                                                          2. Click ' Update Xlsx DB'  3. Choose Xlsx file</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                       2. Click 'Compare NumCollegeGrads vs NumJobs per state'                        3. Click 'Visualize TXT Format                                                                                      4. Click 'Ascending Order'</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                         2. Click 'Compare NumCollegeGrads vs NumJobs per state'                      3. Click 'Visualize TXT Format'                                                                                  4. Click 'Descenidng Order'</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                            2. Click 'Compare NumCollegeGrads vs NumJobs per state'                         3. Click 'Visualize Map'</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                            2. Click 'Compare 3YearCohortBal vs 25PercentileSalary per state'                          3. Click 'Visualize TXT Format'                                                                                       4. Click 'Descending Order'</t>
+  </si>
+  <si>
+    <t>1. Click 'Visualize'                                                                                                       2. Click 'Compare 3YearCohortBal vs 25PercentileSalary per state'          3. Click 'Visualize Map'</t>
+  </si>
+  <si>
+    <t>Run Program     Update Both Data</t>
+  </si>
+  <si>
+    <t>Table will appear with color coded data with highest data point on top in red and lowest at the bottom in blue</t>
+  </si>
+  <si>
+    <t>Table will appear with color coded data with lowest data point on top in blue and highest at the bottom in red</t>
+  </si>
+  <si>
+    <t>Visualize Grads vs Jobs Map</t>
+  </si>
+  <si>
+    <t>Open Browser and display color coded Map of US, pop up task accomplished</t>
+  </si>
+  <si>
+    <t>Display the correct data with correct color in correct order, pop up task accomplished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Browser should open and display color coded map of US, red being highest ratio, blue being lowest. </t>
+  </si>
+  <si>
+    <t>Manual GUI Tests</t>
   </si>
 </sst>
 </file>
@@ -107,9 +191,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
@@ -391,17 +479,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:E9"/>
+  <dimension ref="A4:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -414,39 +503,182 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>